<commit_message>
Add Create method that generates test data and store data into data source
</commit_message>
<xml_diff>
--- a/target/classes/TestData/TestData.xlsx
+++ b/target/classes/TestData/TestData.xlsx
@@ -3,20 +3,21 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr defaultThemeVersion="153222"/>
-  <mc:AlternateContent>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Tahobs\CIB_DigitalTech_UIAutomation\src\main\resources\TestData\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="3795" windowHeight="2760"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="3795" windowHeight="2760" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="UserDetails" sheetId="1" r:id="rId1"/>
+    <sheet name="Sheet1" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="152511"/>
   <extLst>
-    <ext uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
   </extLst>
@@ -24,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="6">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="12">
   <si>
     <t>Name</t>
   </si>
@@ -42,20 +43,43 @@
   </si>
   <si>
     <t>USA</t>
+  </si>
+  <si>
+    <t>firstName</t>
+  </si>
+  <si>
+    <t>lastName</t>
+  </si>
+  <si>
+    <t>userName</t>
+  </si>
+  <si>
+    <t>password</t>
+  </si>
+  <si>
+    <t>email</t>
+  </si>
+  <si>
+    <t>mobileNumber</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <numFmts count="0"/>
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="9.8000000000000007"/>
+      <color rgb="FF000000"/>
+      <name val="Consolas"/>
+      <family val="3"/>
     </font>
   </fonts>
   <fills count="2">
@@ -78,8 +102,11 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -362,7 +389,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B4"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="G13" sqref="G13"/>
     </sheetView>
   </sheetViews>
@@ -376,7 +403,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>2</v>
       </c>
@@ -384,7 +411,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="3">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>2</v>
       </c>
@@ -392,12 +419,54 @@
         <v>3</v>
       </c>
     </row>
-    <row r="4">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>4</v>
       </c>
       <c r="B4" t="s">
         <v>5</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:F1"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="I6" sqref="I6"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="10" bestFit="1" customWidth="1"/>
+    <col min="2" max="4" width="9" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="6" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="13.140625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>11</v>
       </c>
     </row>
   </sheetData>

</xml_diff>